<commit_message>
task A and some transform changes
</commit_message>
<xml_diff>
--- a/points.xlsx
+++ b/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucliveac-my.sharepoint.com/personal/dmc284_uclive_ac_nz/Documents/2025/ENMT482/Assignment 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{6E1EF13E-EF91-497D-9452-7E18C2F07B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2058C4AC-F6E4-4897-AEAC-1F5DB1DEFBCC}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{6E1EF13E-EF91-497D-9452-7E18C2F07B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B4DF5B4-5AFF-4EB5-8095-8018396242E2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{E8225CB9-45CE-4437-8AC0-83402CB2D7CC}"/>
   </bookViews>
@@ -4059,7 +4059,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5448,7 +5448,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -5765,6 +5765,7 @@
     <filterColumn colId="3">
       <filters>
         <filter val="mazzer"/>
+        <filter val="rancilio_tool"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>